<commit_message>
Stored Evaluations in excel file , created rag pipeline
</commit_message>
<xml_diff>
--- a/Evaluations.xlsx
+++ b/Evaluations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Abdullah Files\Programmming\python\IslamQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9E4490-3608-49E1-B73F-CA55A18CBAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74218A72-4B37-45F4-B1EA-E91EC03C515B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Model</t>
   </si>
@@ -49,6 +49,24 @@
   </si>
   <si>
     <t>Average ROUGE-L F1</t>
+  </si>
+  <si>
+    <t>deepseek_r1_distill_llama_70b</t>
+  </si>
+  <si>
+    <t>deepseek-r1t2-chimera.jsonl</t>
+  </si>
+  <si>
+    <t>gemini</t>
+  </si>
+  <si>
+    <t>llama-4-maverick-17b-128e-instruct</t>
+  </si>
+  <si>
+    <t>Mistral-7b (temperature = 0.1)</t>
+  </si>
+  <si>
+    <t>phi4</t>
   </si>
 </sst>
 </file>
@@ -372,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,13 +473,253 @@
       <c r="S3" s="2"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.78539999999999999</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>0.81830000000000003</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2">
+        <v>0.80130000000000001</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2">
+        <v>0.1067</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2">
+        <v>5.9900000000000002E-2</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>0.82040000000000002</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2">
+        <v>0.78979999999999995</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2">
+        <v>0.109</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2">
+        <v>6.1800000000000001E-2</v>
+      </c>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.76949999999999996</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>0.82689999999999997</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2">
+        <v>8.5699999999999998E-2</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2">
+        <v>1.84E-2</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2">
+        <v>1.5299999999999999E-2</v>
+      </c>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.78990000000000005</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>0.82509999999999994</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
+        <v>0.80679999999999996</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2">
+        <v>0.1245</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2">
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2">
+        <v>7.5200000000000003E-2</v>
+      </c>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.80349999999999999</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>0.82489999999999997</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2">
+        <v>0.81369999999999998</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2">
+        <v>0.14879999999999999</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2">
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2">
+        <v>9.01E-2</v>
+      </c>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.77310000000000001</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2">
+        <v>0.81510000000000005</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2">
+        <v>0.79320000000000002</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2">
+        <v>4.2799999999999998E-2</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2">
+        <v>2.7900000000000001E-2</v>
+      </c>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="48">
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:P4"/>
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B3:D3"/>

</xml_diff>

<commit_message>
RAGAS Rouge, BertScore for Mistral Rag computed
</commit_message>
<xml_diff>
--- a/Evaluations.xlsx
+++ b/Evaluations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Abdullah Files\Programmming\python\IslamQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDFA94B-34F2-4C14-B58E-F8264F656F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A032D89-4449-4179-B622-228B2174D374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Model</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t xml:space="preserve">Quran RAG </t>
+  </si>
+  <si>
+    <t>faithfulness</t>
+  </si>
+  <si>
+    <t>answer_relevancy</t>
+  </si>
+  <si>
+    <t>context_precision</t>
+  </si>
+  <si>
+    <t>context_recall</t>
   </si>
 </sst>
 </file>
@@ -113,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -125,6 +137,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -407,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W13"/>
+  <dimension ref="A1:AE13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AC13" sqref="AC13:AE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,7 +434,7 @@
     <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -444,7 +459,7 @@
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,8 +493,28 @@
       </c>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -514,7 +549,7 @@
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -549,7 +584,7 @@
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -584,7 +619,7 @@
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -619,7 +654,7 @@
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -654,7 +689,7 @@
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -689,7 +724,7 @@
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -724,7 +759,7 @@
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -751,43 +786,69 @@
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>0.82240000000000002</v>
+        <v>0.82250000000000001</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2">
-        <v>0.82279999999999998</v>
+        <v>0.82220000000000004</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2">
-        <v>0.82220000000000004</v>
+        <v>0.82189999999999996</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2">
-        <v>0.16869999999999999</v>
+        <v>0.16270000000000001</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2">
-        <v>2.6599999999999999E-2</v>
+        <v>2.53E-2</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2">
-        <v>0.1057</v>
+        <v>0.10249999999999999</v>
       </c>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
+      <c r="T13" s="2">
+        <v>2.8500000000000001E-2</v>
+      </c>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2">
+        <v>0.35270000000000001</v>
+      </c>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2">
+        <v>0.14419999999999999</v>
+      </c>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2">
+        <v>0.1676</v>
+      </c>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="56">
+  <mergeCells count="64">
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="T13:V13"/>
+    <mergeCell ref="W13:Y13"/>
+    <mergeCell ref="Z13:AB13"/>
+    <mergeCell ref="AC13:AE13"/>
     <mergeCell ref="A1:W1"/>
     <mergeCell ref="A12:W12"/>
     <mergeCell ref="B13:D13"/>
@@ -796,6 +857,8 @@
     <mergeCell ref="K13:M13"/>
     <mergeCell ref="N13:P13"/>
     <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="W2:Y2"/>
     <mergeCell ref="N2:P2"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="B4:D4"/>

</xml_diff>

<commit_message>
Sorry to not commit deepseek , llama , gemini done with evaluation and evaluation file is updated but i am not sure about the result
</commit_message>
<xml_diff>
--- a/Evaluations.xlsx
+++ b/Evaluations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Abdullah Files\Programmming\python\IslamQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A032D89-4449-4179-B622-228B2174D374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8BD6B9-2ABC-4E26-BE5E-20EF61D8DA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Model</t>
   </si>
@@ -82,13 +82,19 @@
   </si>
   <si>
     <t>context_recall</t>
+  </si>
+  <si>
+    <t>MERGED RAG</t>
+  </si>
+  <si>
+    <t>llama</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +104,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -125,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -136,10 +150,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -422,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE13"/>
+  <dimension ref="A1:AE18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13:AE13"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,12 +504,12 @@
       </c>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
-      <c r="W2" s="5" t="s">
+      <c r="W2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="X2" s="3"/>
@@ -628,11 +639,11 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>0.82689999999999997</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="2">
         <v>0.79700000000000004</v>
       </c>
@@ -658,71 +669,71 @@
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="4">
         <v>0.78990000000000005</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4">
         <v>0.82509999999999994</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2">
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4">
         <v>0.80679999999999996</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2">
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4">
         <v>0.1245</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2">
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4">
         <v>2.3199999999999998E-2</v>
       </c>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2">
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4">
         <v>7.5200000000000003E-2</v>
       </c>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="3">
         <v>0.80349999999999999</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="2">
         <v>0.82489999999999997</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2">
+      <c r="H9" s="3">
         <v>0.81369999999999998</v>
       </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2">
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3">
         <v>0.14879999999999999</v>
       </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2">
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3">
         <v>2.6200000000000001E-2</v>
       </c>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2">
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3">
         <v>9.01E-2</v>
       </c>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -763,31 +774,39 @@
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2">
@@ -841,48 +860,177 @@
       <c r="AD13" s="2"/>
       <c r="AE13" s="2"/>
     </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.82879999999999998</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2">
+        <v>0.80769999999999997</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2">
+        <v>0.81789999999999996</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2">
+        <v>4.2099999999999999E-2</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2">
+        <v>3.85E-2</v>
+      </c>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.80840000000000001</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2">
+        <v>0.80979999999999996</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2">
+        <v>0.80879999999999996</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2">
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2">
+        <v>5.3800000000000001E-2</v>
+      </c>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.79059999999999997</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2">
+        <v>0.81940000000000002</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2">
+        <v>0.80449999999999999</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2">
+        <v>0.11550000000000001</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2">
+        <v>1.12E-2</v>
+      </c>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2">
+        <v>6.4100000000000004E-2</v>
+      </c>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="64">
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="T13:V13"/>
-    <mergeCell ref="W13:Y13"/>
-    <mergeCell ref="Z13:AB13"/>
-    <mergeCell ref="AC13:AE13"/>
-    <mergeCell ref="A1:W1"/>
-    <mergeCell ref="A12:W12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N5:P5"/>
+  <mergeCells count="83">
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="A15:AE15"/>
+    <mergeCell ref="A12:AE12"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="E10:G10"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="E9:G9"/>
@@ -898,15 +1046,45 @@
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="N7:P7"/>
     <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="T13:V13"/>
+    <mergeCell ref="W13:Y13"/>
+    <mergeCell ref="Z13:AB13"/>
+    <mergeCell ref="AC13:AE13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>